<commit_message>
working on analysis for 20190814 test
</commit_message>
<xml_diff>
--- a/code/processing/growth_curves_plate_reader/20190814_r1_O2_selection_test/20190814_plate_layout.xlsx
+++ b/code/processing/growth_curves_plate_reader/20190814_r1_O2_selection_test/20190814_plate_layout.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19440" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="strains" sheetId="1" r:id="rId1"/>
+    <sheet name="strain" sheetId="1" r:id="rId1"/>
     <sheet name="well" sheetId="5" r:id="rId2"/>
     <sheet name="media" sheetId="2" r:id="rId3"/>
     <sheet name="challenge" sheetId="3" r:id="rId4"/>
@@ -727,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1692,7 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
partial qualitative analysis of dataset. Phenotypes behave more or less as expected
</commit_message>
<xml_diff>
--- a/code/processing/growth_curves_plate_reader/20190814_r1_O2_selection_test/20190814_plate_layout.xlsx
+++ b/code/processing/growth_curves_plate_reader/20190814_r1_O2_selection_test/20190814_plate_layout.xlsx
@@ -398,12 +398,6 @@
     <t>0.2% 2-DODG</t>
   </si>
   <si>
-    <t>pZS2*5-O1+11-sacB-tetA-gfp</t>
-  </si>
-  <si>
-    <t>pZS2*5-O1+11-galK-tetA-gfp</t>
-  </si>
-  <si>
     <t>tetA</t>
   </si>
   <si>
@@ -411,6 +405,12 @@
   </si>
   <si>
     <t>galK</t>
+  </si>
+  <si>
+    <t>pZS2*5-O2+11-sacB-tetA-gfp</t>
+  </si>
+  <si>
+    <t>pZS2*5-O2+11-galK-tetA-gfp</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection sqref="A1:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2034,13 +2034,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -2052,13 +2052,13 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2072,13 +2072,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
@@ -2090,13 +2090,13 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2110,13 +2110,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
@@ -2128,13 +2128,13 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2148,13 +2148,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
@@ -2166,13 +2166,13 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2186,13 +2186,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
@@ -2224,13 +2224,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
@@ -2242,13 +2242,13 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2262,13 +2262,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
@@ -2280,13 +2280,13 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2300,13 +2300,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -2318,13 +2318,13 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="L8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2337,7 +2337,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2353,13 +2353,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -2371,13 +2371,13 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2391,13 +2391,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
@@ -2409,13 +2409,13 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2429,13 +2429,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
@@ -2447,13 +2447,13 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2467,13 +2467,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
@@ -2485,13 +2485,13 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2505,13 +2505,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
@@ -2543,13 +2543,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
@@ -2561,13 +2561,13 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2581,13 +2581,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
@@ -2599,13 +2599,13 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2619,13 +2619,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -2637,13 +2637,13 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2672,13 +2672,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -2690,13 +2690,13 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2710,13 +2710,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
@@ -2728,13 +2728,13 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2748,13 +2748,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
@@ -2766,13 +2766,13 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2786,13 +2786,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
@@ -2804,13 +2804,13 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2824,13 +2824,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
@@ -2862,13 +2862,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
@@ -2880,13 +2880,13 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2900,13 +2900,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
@@ -2918,13 +2918,13 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2938,13 +2938,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -2956,13 +2956,13 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>